<commit_message>
FINALLY, JEESUS CHRIST. LA HAUTEUR VARIABLE FONCTIONNE.
</commit_message>
<xml_diff>
--- a/B65_-_Automne_2018_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
+++ b/B65_-_Automne_2018_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurier\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Git repos\projet_synthese_hiver_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195" tabRatio="494" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="9195" tabRatio="494" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Planification" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="92">
   <si>
     <t>No</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>sprint 3</t>
+  </si>
+  <si>
+    <t>développement du plancher à hauteur dynamique</t>
   </si>
 </sst>
 </file>
@@ -1494,68 +1497,6 @@
   </cellStyles>
   <dxfs count="82">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCDEE0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <top style="thin">
-          <color rgb="FFC00000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFC00000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFC00000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFC00000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2407,11 +2348,61 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCDEE0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
         <color rgb="FFC00000"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <top style="thin">
+          <color rgb="FFC00000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFC00000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFC00000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFC00000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2536,6 +2527,18 @@
           </stop>
         </gradientFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2700,7 +2703,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -2718,8 +2721,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="443853376"/>
-        <c:axId val="443854944"/>
+        <c:axId val="-1901180192"/>
+        <c:axId val="-1901184000"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2792,11 +2795,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="443853376"/>
-        <c:axId val="443854944"/>
+        <c:axId val="-1901180192"/>
+        <c:axId val="-1901184000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="443853376"/>
+        <c:axId val="-1901180192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2839,7 +2842,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443854944"/>
+        <c:crossAx val="-1901184000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2847,7 +2850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443854944"/>
+        <c:axId val="-1901184000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2898,7 +2901,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443853376"/>
+        <c:crossAx val="-1901180192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3113,7 +3116,7 @@
                   <c:v>29.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.75</c:v>
+                  <c:v>26.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.25</c:v>
@@ -3181,7 +3184,7 @@
                   <c:v>33.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3200,11 +3203,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-15"/>
-        <c:axId val="443852984"/>
-        <c:axId val="443853768"/>
+        <c:axId val="-1901191616"/>
+        <c:axId val="-1901192160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="443852984"/>
+        <c:axId val="-1901191616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3247,7 +3250,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443853768"/>
+        <c:crossAx val="-1901192160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3255,7 +3258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443853768"/>
+        <c:axId val="-1901192160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3306,7 +3309,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443852984"/>
+        <c:crossAx val="-1901191616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3592,7 +3595,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -3694,7 +3697,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -4019,7 +4022,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4121,7 +4124,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -6872,8 +6875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AJ90"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6938,7 +6941,7 @@
       <c r="G5" s="29"/>
       <c r="H5" s="60" t="str">
         <f>IF(L44=0,CONCATENATE(AE12, " totalisant ", AE15, " de travail estimé."),CONCATENATE("Attention, il reste " &amp; L45 &amp; " à remplir."))</f>
-        <v>18 tâches ont été définies totalisant 53 heures et 15 minutes de travail estimé.</v>
+        <v>19 tâches ont été définies totalisant 61 heures et 15 minutes de travail estimé.</v>
       </c>
     </row>
     <row r="6" spans="2:31" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -7021,7 +7024,7 @@
       </c>
       <c r="U8" s="3">
         <f>MAX(B8:B42)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V8" s="3" t="s">
         <v>19</v>
@@ -7047,11 +7050,11 @@
       </c>
       <c r="AC8" s="4">
         <f>COUNTA(C8:C43)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AD8" s="9">
         <f>SUM(G8:G43)</f>
-        <v>2.218750000000004</v>
+        <v>2.552083333333337</v>
       </c>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
@@ -7126,7 +7129,7 @@
       </c>
       <c r="AD9" s="10">
         <f>AD8</f>
-        <v>2.218750000000004</v>
+        <v>2.552083333333337</v>
       </c>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
@@ -7198,7 +7201,7 @@
       </c>
       <c r="AD10" s="63">
         <f>DAY(AD8)*24+HOUR(AD8)</f>
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
@@ -7323,11 +7326,11 @@
       </c>
       <c r="AD12" s="4">
         <f>AC8</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE12" s="4" t="str">
         <f>AD12 &amp; " " &amp; AC12 &amp; IF(AD12 &gt; 1, "s ont été définies", " a été définie")</f>
-        <v>18 tâches ont été définies</v>
+        <v>19 tâches ont été définies</v>
       </c>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
@@ -7393,11 +7396,11 @@
       </c>
       <c r="AD13" s="4">
         <f>AD10</f>
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="AE13" s="4" t="str">
         <f>AD13 &amp; " " &amp; AC13 &amp; IF(AD13 &gt; 1, "s", "")</f>
-        <v>53 heures</v>
+        <v>61 heures</v>
       </c>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
@@ -7524,7 +7527,7 @@
       </c>
       <c r="AE15" s="4" t="str">
         <f>IF(AD13&gt;0,IF(AD14&gt;0,AE13&amp;" et "&amp;AE14,AE13),AE14)</f>
-        <v>53 heures et 15 minutes</v>
+        <v>61 heures et 15 minutes</v>
       </c>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
@@ -7735,15 +7738,15 @@
       </c>
       <c r="AD18" s="4">
         <f t="array" ref="AD18">SUM(($H$8:$H$42=$AC18)*$G$8:$G$42)</f>
-        <v>0.78125000000000167</v>
+        <v>1.1145833333333346</v>
       </c>
       <c r="AE18" s="4">
         <f>AD18 * 24*60</f>
-        <v>1125.0000000000023</v>
+        <v>1605.0000000000018</v>
       </c>
       <c r="AF18" s="4">
         <f t="shared" ref="AF18:AF19" si="6">DAY(AD18)*24+HOUR(AD18)</f>
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="AG18" s="4">
         <f t="shared" ref="AG18:AG19" si="7">MINUTE(AD18)</f>
@@ -7751,11 +7754,11 @@
       </c>
       <c r="AH18" s="4" t="str">
         <f t="shared" ref="AH18:AH19" si="8">AF18&amp;"h"&amp;TEXT(AG18,"00")</f>
-        <v>18h45</v>
+        <v>26h45</v>
       </c>
       <c r="AJ18" s="4">
         <f>COUNTIF($H$8:$H$42,AC18)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:36" x14ac:dyDescent="0.25">
@@ -7946,15 +7949,15 @@
       </c>
       <c r="AD21" s="4">
         <f>SUM(AD17:AD19)</f>
-        <v>2.2187500000000044</v>
+        <v>2.5520833333333375</v>
       </c>
       <c r="AE21" s="4">
         <f t="shared" ref="AE21" si="9">AD21 * 24*60</f>
-        <v>3195.0000000000064</v>
+        <v>3675.0000000000059</v>
       </c>
       <c r="AF21" s="4">
         <f t="shared" ref="AF21" si="10">DAY(AD21)*24+HOUR(AD21)</f>
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" ref="AG21" si="11">MINUTE(AD21)</f>
@@ -7962,7 +7965,7 @@
       </c>
       <c r="AH21" s="4" t="str">
         <f t="shared" ref="AH21" si="12">AF21&amp;"h"&amp;TEXT(AG21,"00")</f>
-        <v>53h15</v>
+        <v>61h15</v>
       </c>
     </row>
     <row r="22" spans="2:36" x14ac:dyDescent="0.25">
@@ -8095,23 +8098,23 @@
         <v>90</v>
       </c>
       <c r="L24" s="3" t="b">
-        <f>AND(NOT(ISBLANK($C24)),LEN(D24)=0)</f>
+        <f t="shared" ref="L24:P25" si="13">AND(NOT(ISBLANK($C24)),LEN(D24)=0)</f>
         <v>0</v>
       </c>
       <c r="M24" s="3" t="b">
-        <f>AND(NOT(ISBLANK($C24)),LEN(E24)=0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N24" s="3" t="b">
-        <f>AND(NOT(ISBLANK($C24)),LEN(F24)=0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="O24" s="3" t="b">
-        <f>AND(NOT(ISBLANK($C24)),LEN(G24)=0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P24" s="3" t="b">
-        <f>AND(NOT(ISBLANK($C24)),LEN(H24)=0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T24" s="3">
@@ -8148,23 +8151,23 @@
         <v>90</v>
       </c>
       <c r="L25" s="3" t="b">
-        <f>AND(NOT(ISBLANK($C25)),LEN(D25)=0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M25" s="3" t="b">
-        <f>AND(NOT(ISBLANK($C25)),LEN(E25)=0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N25" s="3" t="b">
-        <f>AND(NOT(ISBLANK($C25)),LEN(F25)=0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="O25" s="3" t="b">
-        <f>AND(NOT(ISBLANK($C25)),LEN(G25)=0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P25" s="3" t="b">
-        <f>AND(NOT(ISBLANK($C25)),LEN(H25)=0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T25" s="3">
@@ -8178,34 +8181,46 @@
       </c>
     </row>
     <row r="26" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="str">
+      <c r="B26" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="42"/>
+        <v>19</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="18">
+        <v>3</v>
+      </c>
+      <c r="G26" s="32">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H26" s="42" t="s">
+        <v>2</v>
+      </c>
       <c r="L26" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M26" s="3" t="b">
-        <f t="shared" ref="M26:M42" si="13">AND(NOT(ISBLANK($C26)),LEN(E26)=0)</f>
+        <f t="shared" ref="M26:M42" si="14">AND(NOT(ISBLANK($C26)),LEN(E26)=0)</f>
         <v>0</v>
       </c>
       <c r="N26" s="3" t="b">
-        <f t="shared" ref="N26:N42" si="14">AND(NOT(ISBLANK($C26)),LEN(F26)=0)</f>
+        <f t="shared" ref="N26:N42" si="15">AND(NOT(ISBLANK($C26)),LEN(F26)=0)</f>
         <v>0</v>
       </c>
       <c r="O26" s="3" t="b">
-        <f t="shared" ref="O26:O42" si="15">AND(NOT(ISBLANK($C26)),LEN(G26)=0)</f>
+        <f t="shared" ref="O26:O42" si="16">AND(NOT(ISBLANK($C26)),LEN(G26)=0)</f>
         <v>0</v>
       </c>
       <c r="P26" s="3" t="b">
-        <f t="shared" ref="P26:P42" si="16">AND(NOT(ISBLANK($C26)),LEN(H26)=0)</f>
+        <f t="shared" ref="P26:P42" si="17">AND(NOT(ISBLANK($C26)),LEN(H26)=0)</f>
         <v>0</v>
       </c>
       <c r="T26" s="3">
@@ -8234,19 +8249,19 @@
         <v>0</v>
       </c>
       <c r="M27" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N27" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O27" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P27" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T27" s="3">
@@ -8275,19 +8290,19 @@
         <v>0</v>
       </c>
       <c r="M28" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N28" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O28" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P28" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T28" s="3">
@@ -8316,19 +8331,19 @@
         <v>0</v>
       </c>
       <c r="M29" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N29" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O29" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P29" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T29" s="3">
@@ -8354,19 +8369,19 @@
         <v>0</v>
       </c>
       <c r="M30" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N30" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O30" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P30" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T30" s="3">
@@ -8392,19 +8407,19 @@
         <v>0</v>
       </c>
       <c r="M31" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N31" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O31" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P31" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T31" s="3">
@@ -8430,19 +8445,19 @@
         <v>0</v>
       </c>
       <c r="M32" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N32" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O32" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P32" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T32" s="3">
@@ -8468,19 +8483,19 @@
         <v>0</v>
       </c>
       <c r="M33" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N33" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O33" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P33" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T33" s="3">
@@ -8506,19 +8521,19 @@
         <v>0</v>
       </c>
       <c r="M34" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N34" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O34" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P34" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T34" s="3">
@@ -8544,19 +8559,19 @@
         <v>0</v>
       </c>
       <c r="M35" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N35" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O35" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P35" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T35" s="3">
@@ -8582,19 +8597,19 @@
         <v>0</v>
       </c>
       <c r="M36" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N36" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O36" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P36" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T36" s="3">
@@ -8620,19 +8635,19 @@
         <v>0</v>
       </c>
       <c r="M37" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N37" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O37" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P37" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T37" s="3">
@@ -8658,19 +8673,19 @@
         <v>0</v>
       </c>
       <c r="M38" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N38" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O38" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P38" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T38" s="3">
@@ -8696,19 +8711,19 @@
         <v>0</v>
       </c>
       <c r="M39" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N39" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O39" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P39" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T39" s="3">
@@ -8734,19 +8749,19 @@
         <v>0</v>
       </c>
       <c r="M40" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N40" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O40" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P40" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T40" s="3">
@@ -8772,19 +8787,19 @@
         <v>0</v>
       </c>
       <c r="M41" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N41" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O41" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P41" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T41" s="3">
@@ -8810,19 +8825,19 @@
         <v>0</v>
       </c>
       <c r="M42" s="3" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N42" s="3" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O42" s="3" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P42" s="3" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T42" s="3">
@@ -8838,19 +8853,19 @@
         <v>0</v>
       </c>
       <c r="M43" s="3">
-        <f t="shared" ref="M43:P43" si="17">COUNTIF(M8:M42,TRUE)</f>
+        <f t="shared" ref="M43:P43" si="18">COUNTIF(M8:M42,TRUE)</f>
         <v>0</v>
       </c>
       <c r="N43" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O43" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P43" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="X43" s="8">
@@ -9108,32 +9123,32 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:H11 B21:H42 B12:B20 D19:H20">
-    <cfRule type="expression" dxfId="3" priority="15">
+    <cfRule type="expression" dxfId="81" priority="15">
       <formula>$E8="Optionnelle"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="17">
+    <cfRule type="expression" dxfId="80" priority="17">
       <formula>$E8="Essentielle"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8 F10 F20 F22 F24 F26 F28 F30 F32 F34 F36 F38 F40 F42">
-    <cfRule type="expression" dxfId="81" priority="25">
+    <cfRule type="expression" dxfId="79" priority="25">
       <formula>$F8=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="27">
+    <cfRule type="expression" dxfId="78" priority="27">
       <formula>$F8=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="29">
+    <cfRule type="expression" dxfId="77" priority="29">
       <formula>$F8=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9 F11 F37 F39 F41 F33:F35 F31 F21:F27 F29 F19">
-    <cfRule type="expression" dxfId="78" priority="24">
+    <cfRule type="expression" dxfId="76" priority="24">
       <formula>$F9=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="26">
+    <cfRule type="expression" dxfId="75" priority="26">
       <formula>$F9=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="28">
+    <cfRule type="expression" dxfId="74" priority="28">
       <formula>$F9=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9166,57 +9181,57 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:G11 D19:G42">
-    <cfRule type="expression" dxfId="4" priority="21">
+    <cfRule type="expression" dxfId="73" priority="21">
       <formula>L8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H11 H19:H42">
-    <cfRule type="expression" dxfId="1" priority="20">
+    <cfRule type="expression" dxfId="72" priority="20">
       <formula>$P8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="75" priority="19">
+    <cfRule type="expression" dxfId="71" priority="19">
       <formula>$L$44&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:H9 B11:H11 B13 B15 B19 B21:H21 B23:H23 B25:H25 B27:H27 B29:H29 B31:H31 B33:H33 B35:H35 B37:H37 B39:H39 B41:H41 B17 D19:H19">
-    <cfRule type="expression" dxfId="0" priority="42">
+    <cfRule type="expression" dxfId="70" priority="42">
       <formula>LEN($B9)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:H8 B10:H10 B12 B14 B16 B20 B22:H22 B24:H24 B26:H26 B28:H28 B30:H30 B32:H32 B34:H34 B36:H36 B38:H38 B40:H40 B42:H42 B18 D20:H20">
-    <cfRule type="expression" dxfId="74" priority="18">
+    <cfRule type="expression" dxfId="69" priority="18">
       <formula>LEN($B8)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:H17 D18:H18 C18:C20">
-    <cfRule type="expression" dxfId="73" priority="1">
+    <cfRule type="expression" dxfId="68" priority="1">
       <formula>$E12="Optionnelle"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="2">
+    <cfRule type="expression" dxfId="67" priority="2">
       <formula>$E12="Essentielle"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12 F14 F16 F18">
-    <cfRule type="expression" dxfId="71" priority="9">
+    <cfRule type="expression" dxfId="66" priority="9">
       <formula>$F12=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="11">
+    <cfRule type="expression" dxfId="65" priority="11">
       <formula>$F12=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="13">
+    <cfRule type="expression" dxfId="64" priority="13">
       <formula>$F12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13:F18">
-    <cfRule type="expression" dxfId="68" priority="8">
+    <cfRule type="expression" dxfId="63" priority="8">
       <formula>$F13=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="10">
+    <cfRule type="expression" dxfId="62" priority="10">
       <formula>$F13=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="12">
+    <cfRule type="expression" dxfId="61" priority="12">
       <formula>$F13=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9249,22 +9264,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:G18">
-    <cfRule type="expression" dxfId="65" priority="5">
+    <cfRule type="expression" dxfId="60" priority="5">
       <formula>L12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H18">
-    <cfRule type="expression" dxfId="64" priority="4">
+    <cfRule type="expression" dxfId="59" priority="4">
       <formula>$P12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:H13 C15:H15 C17:H17 C18:C20">
-    <cfRule type="expression" dxfId="63" priority="14">
+    <cfRule type="expression" dxfId="58" priority="14">
       <formula>LEN($B13)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:H12 C14:H14 C16:H16 D18:H18">
-    <cfRule type="expression" dxfId="62" priority="3">
+    <cfRule type="expression" dxfId="57" priority="3">
       <formula>LEN($B12)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9367,8 +9382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W56"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10109,17 +10124,17 @@
       <c r="P25" s="8"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="53" t="str">
+      <c r="B26" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B26)&lt;&gt;0,'Sprint 1 - Planification'!B26,"")</f>
-        <v/>
+        <v>19</v>
       </c>
       <c r="C26" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v/>
+        <v>développement du plancher à hauteur dynamique</v>
       </c>
       <c r="D26" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E26" s="118"/>
       <c r="F26" s="116"/>
@@ -10687,97 +10702,97 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:D42">
-    <cfRule type="expression" dxfId="61" priority="10">
+    <cfRule type="expression" dxfId="56" priority="10">
       <formula>$F8=100%</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="11">
+    <cfRule type="expression" dxfId="55" priority="11">
       <formula>$D8&lt;&gt;"Sprint 1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:G20 E22:G22 E24:G24 E26:G26 E28:G28 E30:G30 E32:G32 E34:G34 E36:G36 E38:G38 E40:G40 E42:G42">
-    <cfRule type="expression" dxfId="59" priority="22">
+    <cfRule type="expression" dxfId="54" priority="22">
       <formula>AND($D20&lt;&gt;"Sprint 1",$F20&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="24">
+    <cfRule type="expression" dxfId="53" priority="24">
       <formula>AND($D20="Sprint 1",$F20&lt;1,NOT(ISBLANK($F20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:G19 E21:G21 E23:G23 E25:G25 E27:G27 E29:G29 E31:G31 E33:G33 E35:G35 E37:G37 E39:G39 E41:G41">
-    <cfRule type="expression" dxfId="57" priority="19">
+    <cfRule type="expression" dxfId="52" priority="19">
       <formula>AND($D19&lt;&gt;"Sprint 1",$F19&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="21">
+    <cfRule type="expression" dxfId="51" priority="21">
       <formula>AND($D19="Sprint 1",$F19&lt;1,NOT(ISBLANK($F19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G42">
-    <cfRule type="expression" dxfId="55" priority="16">
+    <cfRule type="expression" dxfId="50" priority="16">
       <formula>$M19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:E42">
-    <cfRule type="expression" dxfId="54" priority="14">
+    <cfRule type="expression" dxfId="49" priority="14">
       <formula>$K19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:F42">
-    <cfRule type="expression" dxfId="53" priority="13">
+    <cfRule type="expression" dxfId="48" priority="13">
       <formula>$L19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="52" priority="12">
+    <cfRule type="expression" dxfId="47" priority="12">
       <formula>$K$44&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:D8 B10:D10 B12:D12 B14:D14 B16:D16 B18:D18 B20:G20 B22:G22 B24:G24 B26:G26 B28:G28 B30:G30 B32:G32 B34:G34 B36:G36 B38:G38 B40:G40 B42:G42">
-    <cfRule type="expression" dxfId="51" priority="25">
+    <cfRule type="expression" dxfId="46" priority="25">
       <formula>LEN($B8)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:D9 B11:D11 B13:D13 B15:D15 B17:D17 B19:G19 B21:G21 B23:G23 B25:G25 B27:G27 B29:G29 B31:G31 B33:G33 B35:G35 B37:G37 B39:G39 B41:G41">
-    <cfRule type="expression" dxfId="50" priority="20">
+    <cfRule type="expression" dxfId="45" priority="20">
       <formula>LEN($B9)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:G8 E10:G10 E12:G12 E14:G14 E16:G16 E18:G18">
-    <cfRule type="expression" dxfId="49" priority="7">
+    <cfRule type="expression" dxfId="44" priority="7">
       <formula>AND($D8&lt;&gt;"Sprint 1",$F8&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="8">
+    <cfRule type="expression" dxfId="43" priority="8">
       <formula>AND($D8="Sprint 1",$F8&lt;1,NOT(ISBLANK($F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:G9 E11:G11 E13:G13 E15:G15 E17:G17">
-    <cfRule type="expression" dxfId="47" priority="4">
+    <cfRule type="expression" dxfId="42" priority="4">
       <formula>AND($D9&lt;&gt;"Sprint 1",$F9&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="6">
+    <cfRule type="expression" dxfId="41" priority="6">
       <formula>AND($D9="Sprint 1",$F9&lt;1,NOT(ISBLANK($F9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G18">
-    <cfRule type="expression" dxfId="45" priority="3">
+    <cfRule type="expression" dxfId="40" priority="3">
       <formula>$M8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:E18">
-    <cfRule type="expression" dxfId="44" priority="2">
+    <cfRule type="expression" dxfId="39" priority="2">
       <formula>$K8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:F18">
-    <cfRule type="expression" dxfId="43" priority="1">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>$L8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:G8 E10:G10 E12:G12 E14:G14 E16:G16 E18:G18">
-    <cfRule type="expression" dxfId="42" priority="9">
+    <cfRule type="expression" dxfId="37" priority="9">
       <formula>LEN($B8)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:G9 E11:G11 E13:G13 E15:G15 E17:G17">
-    <cfRule type="expression" dxfId="41" priority="5">
+    <cfRule type="expression" dxfId="36" priority="5">
       <formula>LEN($B9)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10805,8 +10820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z57"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10968,7 +10983,7 @@
       </c>
       <c r="V9" s="9">
         <f>SUM(G9:G43)</f>
-        <v>0</v>
+        <v>0.66666666666667596</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
@@ -11016,15 +11031,15 @@
       </c>
       <c r="S10" s="61">
         <f t="array" ref="S10">SUM(($D$9:$D$43=$R10)*$G$9:$G$43)</f>
-        <v>0</v>
+        <v>0.66666666666667596</v>
       </c>
       <c r="T10" s="62">
         <f t="shared" ref="T10:T11" si="4">S10*24*60</f>
-        <v>0</v>
+        <v>960.00000000001342</v>
       </c>
       <c r="V10" s="10">
         <f>V9</f>
-        <v>0</v>
+        <v>0.66666666666667596</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -11080,7 +11095,7 @@
       </c>
       <c r="V11" s="63">
         <f>DAY(V9)*24+HOUR(V9)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -11176,11 +11191,11 @@
       </c>
       <c r="V13" s="63">
         <f>V11</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W13" s="4" t="str">
         <f>V13 &amp; " " &amp; U13 &amp; IF(V13 &gt; 1, "s", "")</f>
-        <v>0 heure</v>
+        <v>16 heures</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
@@ -11279,11 +11294,11 @@
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
         <f>IF(V13&gt;0,IF(V14&gt;0,W13&amp;" et "&amp;W14,W13),W14)</f>
-        <v>0 minute</v>
+        <v>16 heures</v>
       </c>
       <c r="Y15" s="4" t="str">
         <f>V13&amp;"h"&amp;TEXT(V14,"00")</f>
-        <v>0h00</v>
+        <v>16h00</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
@@ -11758,17 +11773,17 @@
       <c r="R26" s="8"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="53" t="str">
+      <c r="B27" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B26)&lt;&gt;0,'Sprint 1 - Planification'!B26,"")</f>
-        <v/>
+        <v>19</v>
       </c>
       <c r="C27" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v/>
+        <v>développement du plancher à hauteur dynamique</v>
       </c>
       <c r="D27" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E27" s="75" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E26),"",'Sprint 1 - Bilan'!E26)</f>
@@ -11778,8 +11793,12 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F26),"",'Sprint 1 - Bilan'!F26)</f>
         <v/>
       </c>
-      <c r="G27" s="118"/>
-      <c r="H27" s="116"/>
+      <c r="G27" s="118">
+        <v>0.66666666666667596</v>
+      </c>
+      <c r="H27" s="116">
+        <v>1</v>
+      </c>
       <c r="I27" s="117"/>
       <c r="M27" s="3" t="b">
         <f t="shared" si="0"/>
@@ -12551,97 +12570,97 @@
     <mergeCell ref="I7:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="B9:F43">
-    <cfRule type="expression" dxfId="40" priority="10">
+    <cfRule type="expression" dxfId="35" priority="10">
       <formula>OR($F9=100%,$H9=100%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="11">
+    <cfRule type="expression" dxfId="34" priority="11">
       <formula>OR($D9="Sprint 3",AND($D9="Sprint 1",$F9=100%))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21:I21 G23:I23 G25:I25 G27:I27 G29:I29 G31:I31 G33:I33 G35:I35 G37:I37 G39:I39 G41:I41 G43:I43">
-    <cfRule type="expression" dxfId="38" priority="19">
+    <cfRule type="expression" dxfId="33" priority="19">
       <formula>AND($D21="Sprint 3",$H21&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="20">
+    <cfRule type="expression" dxfId="32" priority="20">
       <formula>AND($D21&lt;&gt;"Sprint 3",$H21&lt;1,NOT(ISBLANK($H21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:I20 G22:I22 G24:I24 G26:I26 G28:I28 G30:I30 G32:I32 G34:I34 G36:I36 G38:I38 G40:I40 G42:I42">
-    <cfRule type="expression" dxfId="36" priority="16">
+    <cfRule type="expression" dxfId="31" priority="16">
       <formula>AND($D20="Sprint 3",$H20&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="17">
+    <cfRule type="expression" dxfId="30" priority="17">
       <formula>AND($D20&lt;&gt;"Sprint 3",$H20&lt;1,NOT(ISBLANK($H20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I43">
-    <cfRule type="expression" dxfId="34" priority="15">
+    <cfRule type="expression" dxfId="29" priority="15">
       <formula>$O20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:G43">
-    <cfRule type="expression" dxfId="33" priority="14">
+    <cfRule type="expression" dxfId="28" priority="14">
       <formula>$M20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:H43">
-    <cfRule type="expression" dxfId="32" priority="13">
+    <cfRule type="expression" dxfId="27" priority="13">
       <formula>$N20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="31" priority="12">
+    <cfRule type="expression" dxfId="26" priority="12">
       <formula>$M$45&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:F9 B11:F11 B13:F13 B15:F15 B17:F17 B19:F19 B21:I21 B23:I23 B25:I25 B27:I27 B29:I29 B31:I31 B33:I33 B35:I35 B37:I37 B39:I39 B41:I41 B43:I43">
-    <cfRule type="expression" dxfId="30" priority="21">
+    <cfRule type="expression" dxfId="25" priority="21">
       <formula>LEN($B9)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:F10 B12:F12 B14:F14 B16:F16 B18:F18 B20:I20 B22:I22 B24:I24 B26:I26 B28:I28 B30:I30 B32:I32 B34:I34 B36:I36 B38:I38 B40:I40 B42:I42">
-    <cfRule type="expression" dxfId="29" priority="18">
+    <cfRule type="expression" dxfId="24" priority="18">
       <formula>LEN($B10)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:I9 G11:I11 G13:I13 G15:I15 G17:I17 G19:I19">
-    <cfRule type="expression" dxfId="28" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>AND($D9="Sprint 3",$H9&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>AND($D9&lt;&gt;"Sprint 3",$H9&lt;1,NOT(ISBLANK($H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:I10 G12:I12 G14:I14 G16:I16 G18:I18">
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="21" priority="4">
       <formula>AND($D10="Sprint 3",$H10&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>AND($D10&lt;&gt;"Sprint 3",$H10&lt;1,NOT(ISBLANK($H10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I19">
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>$O9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G19">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$M9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H19">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>$N9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:I9 G11:I11 G13:I13 G15:I15 G17:I17 G19:I19">
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>LEN($B9)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:I10 G12:I12 G14:I14 G16:I16 G18:I18">
-    <cfRule type="expression" dxfId="20" priority="6">
+    <cfRule type="expression" dxfId="15" priority="6">
       <formula>LEN($B10)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13630,25 +13649,25 @@
       <c r="R26" s="8"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="53" t="str">
+      <c r="B27" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B26)&lt;&gt;0,'Sprint 1 - Planification'!B26,"")</f>
-        <v/>
+        <v>19</v>
       </c>
       <c r="C27" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v/>
+        <v>développement du plancher à hauteur dynamique</v>
       </c>
       <c r="D27" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
-        <v/>
-      </c>
-      <c r="E27" s="75" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E27" s="75">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E27)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G27)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E27)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G27))</f>
-        <v/>
-      </c>
-      <c r="F27" s="79" t="str">
+        <v>0.66666666666667596</v>
+      </c>
+      <c r="F27" s="79">
         <f>IF(LEN('Sprint 2 - Bilan'!$H27)&lt;&gt;0,'Sprint 2 - Bilan'!$H27,IF(LEN('Sprint 2 - Bilan'!$F27)=0,"",'Sprint 2 - Bilan'!$F27))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G27" s="118"/>
       <c r="H27" s="116"/>
@@ -14423,50 +14442,50 @@
     <mergeCell ref="I7:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="B9:F43">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>OR($F9=100%,$H9=100%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND($D9&lt;&gt;"Sprint 3",$F9=100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:I9 G11:I11 G13:I13 G15:I15 G17:I17 G19:I19 G21:I21 G23:I23 G25:I25 G27:I27 G29:I29 G31:I31 G33:I33 G35:I35 G37:I37 G39:I39 G41:I41 G43:I43">
-    <cfRule type="expression" dxfId="17" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>IF(ISBLANK($H9),IF(ISBLANK($F9),TRUE,$F9&lt;100%),$H9&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:I10 G12:I12 G14:I14 G16:I16 G18:I18 G20:I20 G22:I22 G24:I24 G26:I26 G28:I28 G30:I30 G32:I32 G34:I34 G36:I36 G38:I38 G40:I40 G42:I42">
-    <cfRule type="expression" dxfId="16" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>IF(ISBLANK($H10),IF(ISBLANK($F10),TRUE,$F10&lt;100%),$H10&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I43">
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>$O9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G43">
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$M9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H43">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>$N9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$M$45&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:I9 B11:I11 B13:I13 B15:I15 B17:I17 B19:I19 B21:I21 B23:I23 B25:I25 B27:I27 B29:I29 B31:I31 B33:I33 B35:I35 B37:I37 B39:I39 B41:I41 B43:I43">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>LEN($B9)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:I10 B12:I12 B14:I14 B16:I16 B18:I18 B20:I20 B22:I22 B24:I24 B26:I26 B28:I28 B30:I30 B32:I32 B34:I34 B36:I36 B38:I38 B40:I40 B42:I42">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>LEN($B10)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14591,7 +14610,7 @@
       </c>
       <c r="D8" s="96">
         <f>M8</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="97">
         <f>N8</f>
@@ -14599,7 +14618,7 @@
       </c>
       <c r="F8" s="101">
         <f>O8</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -14609,7 +14628,7 @@
       </c>
       <c r="M8" s="1">
         <f>'Sprint 1 - Planification'!AJ18</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N8" s="1">
         <f>'Sprint 1 - Planification'!AJ19</f>
@@ -14617,7 +14636,7 @@
       </c>
       <c r="O8" s="1">
         <f>SUM(L8:N8)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -14634,7 +14653,7 @@
       </c>
       <c r="D9" s="99" t="str">
         <f t="shared" si="0"/>
-        <v>18h45</v>
+        <v>26h45</v>
       </c>
       <c r="E9" s="100" t="str">
         <f t="shared" si="0"/>
@@ -14642,7 +14661,7 @@
       </c>
       <c r="F9" s="102" t="str">
         <f t="shared" si="0"/>
-        <v>53h15</v>
+        <v>61h15</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -14652,7 +14671,7 @@
       </c>
       <c r="M9" s="1">
         <f>'Sprint 1 - Planification'!AD18</f>
-        <v>0.78125000000000167</v>
+        <v>1.1145833333333346</v>
       </c>
       <c r="N9" s="1">
         <f>'Sprint 1 - Planification'!AD19</f>
@@ -14660,7 +14679,7 @@
       </c>
       <c r="O9" s="1">
         <f>SUM(L9:N9)</f>
-        <v>2.2187500000000044</v>
+        <v>2.5520833333333375</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>66</v>
@@ -14671,7 +14690,7 @@
       </c>
       <c r="R9" s="1">
         <f t="shared" si="1"/>
-        <v>18.75</v>
+        <v>26.75</v>
       </c>
       <c r="S9" s="1">
         <f t="shared" si="1"/>
@@ -14682,7 +14701,7 @@
       </c>
       <c r="V9" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!E8:E42,"Essentielle")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>70</v>
@@ -14702,7 +14721,7 @@
       </c>
       <c r="D10" s="96" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>16h00</v>
       </c>
       <c r="E10" s="97" t="str">
         <f t="shared" si="0"/>
@@ -14710,7 +14729,7 @@
       </c>
       <c r="F10" s="101" t="str">
         <f t="shared" si="0"/>
-        <v>33h15</v>
+        <v>49h15</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -14720,7 +14739,7 @@
       </c>
       <c r="M10" s="1">
         <f>'Sprint 2 - Bilan'!V9</f>
-        <v>0</v>
+        <v>0.66666666666667596</v>
       </c>
       <c r="N10" s="1">
         <f>'Sprint 3 - Bilan'!V9</f>
@@ -14728,7 +14747,7 @@
       </c>
       <c r="O10" s="1">
         <f>SUM(L10:N10)</f>
-        <v>1.3854166666666681</v>
+        <v>2.0520833333333441</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>67</v>
@@ -14739,7 +14758,7 @@
       </c>
       <c r="R10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" si="1"/>
@@ -14807,7 +14826,7 @@
       </c>
       <c r="Y11" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!F8:F42,3)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:25" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -14929,7 +14948,7 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ZTHIqTmr8cTliRMGAcUcmM0mjbf6CIJ0mHH1g8KtGLF4lRA/UYuFPwpT4A16q2cQqIx/6PesESjQGKIAV9ov5g==" saltValue="9FKXXuq3MsinQZgjNrQSTw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="F5:J5">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15252,22 +15271,22 @@
     <mergeCell ref="C35:G35"/>
   </mergeCells>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="8" priority="69">
+    <cfRule type="expression" dxfId="3" priority="69">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fin de la soiree. beaucoup d'avancements ce soir.
</commit_message>
<xml_diff>
--- a/B65_-_Automne_2018_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
+++ b/B65_-_Automne_2018_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="9195" tabRatio="494" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="9195" tabRatio="494" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Planification" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="94">
   <si>
     <t>No</t>
   </si>
@@ -430,7 +430,13 @@
     <t>sprint 3</t>
   </si>
   <si>
-    <t>développement du plancher à hauteur dynamique</t>
+    <t>plancher à hauteur dynamique - collisions</t>
+  </si>
+  <si>
+    <t>plancher à hauteur dynamique - implémentation du "perlin noise"</t>
+  </si>
+  <si>
+    <t>ajout des collisions shère-capsule à l'engin physique</t>
   </si>
 </sst>
 </file>
@@ -2607,6 +2613,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2703,7 +2710,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -2721,8 +2728,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="-1901180192"/>
-        <c:axId val="-1901184000"/>
+        <c:axId val="-1018659632"/>
+        <c:axId val="-1018669968"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2775,10 +2782,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2795,11 +2802,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1901180192"/>
-        <c:axId val="-1901184000"/>
+        <c:axId val="-1018659632"/>
+        <c:axId val="-1018669968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1901180192"/>
+        <c:axId val="-1018659632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2842,7 +2849,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1901184000"/>
+        <c:crossAx val="-1018669968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2850,7 +2857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1901184000"/>
+        <c:axId val="-1018669968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2901,7 +2908,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1901180192"/>
+        <c:crossAx val="-1018659632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2915,6 +2922,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3021,6 +3029,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3116,7 +3125,7 @@
                   <c:v>29.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.75</c:v>
+                  <c:v>34.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.25</c:v>
@@ -3184,7 +3193,7 @@
                   <c:v>33.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3203,11 +3212,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-15"/>
-        <c:axId val="-1901191616"/>
-        <c:axId val="-1901192160"/>
+        <c:axId val="-1012901168"/>
+        <c:axId val="-1012900624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1901191616"/>
+        <c:axId val="-1012901168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3250,7 +3259,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1901192160"/>
+        <c:crossAx val="-1012900624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3258,7 +3267,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1901192160"/>
+        <c:axId val="-1012900624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3309,7 +3318,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1901191616"/>
+        <c:crossAx val="-1012901168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3323,6 +3332,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3429,6 +3439,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3595,7 +3606,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -3697,7 +3708,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -3726,6 +3737,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3832,6 +3844,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4019,7 +4032,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -4124,7 +4137,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -4153,6 +4166,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6941,7 +6955,7 @@
       <c r="G5" s="29"/>
       <c r="H5" s="60" t="str">
         <f>IF(L44=0,CONCATENATE(AE12, " totalisant ", AE15, " de travail estimé."),CONCATENATE("Attention, il reste " &amp; L45 &amp; " à remplir."))</f>
-        <v>19 tâches ont été définies totalisant 61 heures et 15 minutes de travail estimé.</v>
+        <v>21 tâches ont été définies totalisant 69 heures et 15 minutes de travail estimé.</v>
       </c>
     </row>
     <row r="6" spans="2:31" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -7024,7 +7038,7 @@
       </c>
       <c r="U8" s="3">
         <f>MAX(B8:B42)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="V8" s="3" t="s">
         <v>19</v>
@@ -7050,11 +7064,11 @@
       </c>
       <c r="AC8" s="4">
         <f>COUNTA(C8:C43)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AD8" s="9">
         <f>SUM(G8:G43)</f>
-        <v>2.552083333333337</v>
+        <v>2.8854166666666701</v>
       </c>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
@@ -7129,7 +7143,7 @@
       </c>
       <c r="AD9" s="10">
         <f>AD8</f>
-        <v>2.552083333333337</v>
+        <v>2.8854166666666701</v>
       </c>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
@@ -7201,7 +7215,7 @@
       </c>
       <c r="AD10" s="63">
         <f>DAY(AD8)*24+HOUR(AD8)</f>
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
@@ -7326,11 +7340,11 @@
       </c>
       <c r="AD12" s="4">
         <f>AC8</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AE12" s="4" t="str">
         <f>AD12 &amp; " " &amp; AC12 &amp; IF(AD12 &gt; 1, "s ont été définies", " a été définie")</f>
-        <v>19 tâches ont été définies</v>
+        <v>21 tâches ont été définies</v>
       </c>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
@@ -7396,11 +7410,11 @@
       </c>
       <c r="AD13" s="4">
         <f>AD10</f>
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="AE13" s="4" t="str">
         <f>AD13 &amp; " " &amp; AC13 &amp; IF(AD13 &gt; 1, "s", "")</f>
-        <v>61 heures</v>
+        <v>69 heures</v>
       </c>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
@@ -7527,7 +7541,7 @@
       </c>
       <c r="AE15" s="4" t="str">
         <f>IF(AD13&gt;0,IF(AD14&gt;0,AE13&amp;" et "&amp;AE14,AE13),AE14)</f>
-        <v>61 heures et 15 minutes</v>
+        <v>69 heures et 15 minutes</v>
       </c>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
@@ -7738,15 +7752,15 @@
       </c>
       <c r="AD18" s="4">
         <f t="array" ref="AD18">SUM(($H$8:$H$42=$AC18)*$G$8:$G$42)</f>
-        <v>1.1145833333333346</v>
+        <v>1.4479166666666676</v>
       </c>
       <c r="AE18" s="4">
         <f>AD18 * 24*60</f>
-        <v>1605.0000000000018</v>
+        <v>2085.0000000000014</v>
       </c>
       <c r="AF18" s="4">
         <f t="shared" ref="AF18:AF19" si="6">DAY(AD18)*24+HOUR(AD18)</f>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="AG18" s="4">
         <f t="shared" ref="AG18:AG19" si="7">MINUTE(AD18)</f>
@@ -7754,11 +7768,11 @@
       </c>
       <c r="AH18" s="4" t="str">
         <f t="shared" ref="AH18:AH19" si="8">AF18&amp;"h"&amp;TEXT(AG18,"00")</f>
-        <v>26h45</v>
+        <v>34h45</v>
       </c>
       <c r="AJ18" s="4">
         <f>COUNTIF($H$8:$H$42,AC18)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:36" x14ac:dyDescent="0.25">
@@ -7949,15 +7963,15 @@
       </c>
       <c r="AD21" s="4">
         <f>SUM(AD17:AD19)</f>
-        <v>2.5520833333333375</v>
+        <v>2.8854166666666705</v>
       </c>
       <c r="AE21" s="4">
         <f t="shared" ref="AE21" si="9">AD21 * 24*60</f>
-        <v>3675.0000000000059</v>
+        <v>4155.0000000000055</v>
       </c>
       <c r="AF21" s="4">
         <f t="shared" ref="AF21" si="10">DAY(AD21)*24+HOUR(AD21)</f>
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" ref="AG21" si="11">MINUTE(AD21)</f>
@@ -7965,7 +7979,7 @@
       </c>
       <c r="AH21" s="4" t="str">
         <f t="shared" ref="AH21" si="12">AF21&amp;"h"&amp;TEXT(AG21,"00")</f>
-        <v>61h15</v>
+        <v>69h15</v>
       </c>
     </row>
     <row r="22" spans="2:36" x14ac:dyDescent="0.25">
@@ -8234,16 +8248,28 @@
       </c>
     </row>
     <row r="27" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B27" s="45" t="str">
+      <c r="B27" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="41"/>
+        <v>20</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="16">
+        <v>19</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="16">
+        <v>2</v>
+      </c>
+      <c r="G27" s="31">
+        <v>0.125</v>
+      </c>
+      <c r="H27" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="L27" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8275,16 +8301,28 @@
       </c>
     </row>
     <row r="28" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="str">
+      <c r="B28" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="42"/>
+        <v>21</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="18">
+        <v>6</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="18">
+        <v>2</v>
+      </c>
+      <c r="G28" s="32">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="H28" s="42" t="s">
+        <v>2</v>
+      </c>
       <c r="L28" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -10130,7 +10168,7 @@
       </c>
       <c r="C26" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v>développement du plancher à hauteur dynamique</v>
+        <v>plancher à hauteur dynamique - collisions</v>
       </c>
       <c r="D26" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
@@ -10154,17 +10192,17 @@
       <c r="P26" s="8"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="50" t="str">
+      <c r="B27" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B27)&lt;&gt;0,'Sprint 1 - Planification'!B27,"")</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="C27" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C27)&lt;&gt;0,'Sprint 1 - Planification'!C27,"")</f>
-        <v/>
+        <v>plancher à hauteur dynamique - implémentation du "perlin noise"</v>
       </c>
       <c r="D27" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H27)&lt;&gt;0,'Sprint 1 - Planification'!H27,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E27" s="112"/>
       <c r="F27" s="113"/>
@@ -10184,17 +10222,17 @@
       <c r="P27" s="8"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="53" t="str">
+      <c r="B28" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B28)&lt;&gt;0,'Sprint 1 - Planification'!B28,"")</f>
-        <v/>
+        <v>21</v>
       </c>
       <c r="C28" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C28)&lt;&gt;0,'Sprint 1 - Planification'!C28,"")</f>
-        <v/>
+        <v>ajout des collisions shère-capsule à l'engin physique</v>
       </c>
       <c r="D28" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H28)&lt;&gt;0,'Sprint 1 - Planification'!H28,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E28" s="115"/>
       <c r="F28" s="116"/>
@@ -10821,7 +10859,7 @@
   <dimension ref="B1:Z57"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10886,7 +10924,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="64" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 14 champs à remplir!</v>
+        <v>Attention, il reste 16 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -10983,7 +11021,7 @@
       </c>
       <c r="V9" s="9">
         <f>SUM(G9:G43)</f>
-        <v>0.66666666666667596</v>
+        <v>0.7083333333333427</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
@@ -11031,15 +11069,15 @@
       </c>
       <c r="S10" s="61">
         <f t="array" ref="S10">SUM(($D$9:$D$43=$R10)*$G$9:$G$43)</f>
-        <v>0.66666666666667596</v>
+        <v>0.7083333333333427</v>
       </c>
       <c r="T10" s="62">
         <f t="shared" ref="T10:T11" si="4">S10*24*60</f>
-        <v>960.00000000001342</v>
+        <v>1020.0000000000134</v>
       </c>
       <c r="V10" s="10">
         <f>V9</f>
-        <v>0.66666666666667596</v>
+        <v>0.7083333333333427</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -11095,7 +11133,7 @@
       </c>
       <c r="V11" s="63">
         <f>DAY(V9)*24+HOUR(V9)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -11191,11 +11229,11 @@
       </c>
       <c r="V13" s="63">
         <f>V11</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="W13" s="4" t="str">
         <f>V13 &amp; " " &amp; U13 &amp; IF(V13 &gt; 1, "s", "")</f>
-        <v>16 heures</v>
+        <v>17 heures</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
@@ -11294,11 +11332,11 @@
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
         <f>IF(V13&gt;0,IF(V14&gt;0,W13&amp;" et "&amp;W14,W13),W14)</f>
-        <v>16 heures</v>
+        <v>17 heures</v>
       </c>
       <c r="Y15" s="4" t="str">
         <f>V13&amp;"h"&amp;TEXT(V14,"00")</f>
-        <v>16h00</v>
+        <v>17h00</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
@@ -11344,11 +11382,11 @@
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche est en retard!",CONCATENATE(V16," tâches sont en retard!")))</f>
-        <v>7 tâches sont en retard!</v>
+        <v>8 tâches sont en retard!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
@@ -11779,7 +11817,7 @@
       </c>
       <c r="C27" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v>développement du plancher à hauteur dynamique</v>
+        <v>plancher à hauteur dynamique - collisions</v>
       </c>
       <c r="D27" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
@@ -11819,17 +11857,17 @@
       <c r="R27" s="8"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="50" t="str">
+      <c r="B28" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B27)&lt;&gt;0,'Sprint 1 - Planification'!B27,"")</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="C28" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C27)&lt;&gt;0,'Sprint 1 - Planification'!C27,"")</f>
-        <v/>
+        <v>plancher à hauteur dynamique - implémentation du "perlin noise"</v>
       </c>
       <c r="D28" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H27)&lt;&gt;0,'Sprint 1 - Planification'!H27,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E28" s="73" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E27),"",'Sprint 1 - Bilan'!E27)</f>
@@ -11839,8 +11877,12 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F27),"",'Sprint 1 - Bilan'!F27)</f>
         <v/>
       </c>
-      <c r="G28" s="112"/>
-      <c r="H28" s="113"/>
+      <c r="G28" s="112">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H28" s="113">
+        <v>1</v>
+      </c>
       <c r="I28" s="114"/>
       <c r="M28" s="3" t="b">
         <f t="shared" si="0"/>
@@ -11861,17 +11903,17 @@
       <c r="R28" s="8"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="53" t="str">
+      <c r="B29" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B28)&lt;&gt;0,'Sprint 1 - Planification'!B28,"")</f>
-        <v/>
+        <v>21</v>
       </c>
       <c r="C29" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C28)&lt;&gt;0,'Sprint 1 - Planification'!C28,"")</f>
-        <v/>
+        <v>ajout des collisions shère-capsule à l'engin physique</v>
       </c>
       <c r="D29" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H28)&lt;&gt;0,'Sprint 1 - Planification'!H28,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E29" s="74" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E28),"",'Sprint 1 - Bilan'!E28)</f>
@@ -11886,11 +11928,11 @@
       <c r="I29" s="117"/>
       <c r="M29" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O29" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11898,7 +11940,7 @@
       </c>
       <c r="P29" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R29" s="8"/>
     </row>
@@ -12493,11 +12535,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -12505,21 +12547,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>14 champs</v>
+        <v>16 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -12664,7 +12706,7 @@
       <formula>LEN($B10)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations disablePrompts="1" count="7">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nom de tâche trop long" error="Le nom de votre tâche doit être court. _x000a_Un maximum de 72 caractères est mis à votre disposition._x000a_Pour plus de détail, veuillez faire l'ajout de commentaires." promptTitle="Nom de la tâche" prompt="_x000a_Veuillez saisir le nom de la tâche._x000a__x000a_Lorsque pertinent, n'oubliez pas d'ajouter une description de votre tâche sous forme de commentaire." sqref="C9:C43">
       <formula1>0</formula1>
       <formula2>72</formula2>
@@ -12763,7 +12805,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="64" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 20 champs à remplir!</v>
+        <v>Attention, il reste 22 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -13221,11 +13263,11 @@
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche n'a pas été terminée!",CONCATENATE(V16," tâches n'ont pas été terminé!")))</f>
-        <v>10 tâches n'ont pas été terminé!</v>
+        <v>11 tâches n'ont pas été terminé!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
@@ -13655,7 +13697,7 @@
       </c>
       <c r="C27" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v>développement du plancher à hauteur dynamique</v>
+        <v>plancher à hauteur dynamique - collisions</v>
       </c>
       <c r="D27" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
@@ -13691,25 +13733,25 @@
       <c r="R27" s="8"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="50" t="str">
+      <c r="B28" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B27)&lt;&gt;0,'Sprint 1 - Planification'!B27,"")</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="C28" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C27)&lt;&gt;0,'Sprint 1 - Planification'!C27,"")</f>
-        <v/>
+        <v>plancher à hauteur dynamique - implémentation du "perlin noise"</v>
       </c>
       <c r="D28" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H27)&lt;&gt;0,'Sprint 1 - Planification'!H27,"")</f>
-        <v/>
-      </c>
-      <c r="E28" s="73" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E28" s="73">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E28)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G28)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E28)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G28))</f>
-        <v/>
-      </c>
-      <c r="F28" s="77" t="str">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="F28" s="77">
         <f>IF(LEN('Sprint 2 - Bilan'!$H28)&lt;&gt;0,'Sprint 2 - Bilan'!$H28,IF(LEN('Sprint 2 - Bilan'!$F28)=0,"",'Sprint 2 - Bilan'!$F28))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G28" s="112"/>
       <c r="H28" s="113"/>
@@ -13733,17 +13775,17 @@
       <c r="R28" s="8"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="53" t="str">
+      <c r="B29" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B28)&lt;&gt;0,'Sprint 1 - Planification'!B28,"")</f>
-        <v/>
+        <v>21</v>
       </c>
       <c r="C29" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C28)&lt;&gt;0,'Sprint 1 - Planification'!C28,"")</f>
-        <v/>
+        <v>ajout des collisions shère-capsule à l'engin physique</v>
       </c>
       <c r="D29" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H28)&lt;&gt;0,'Sprint 1 - Planification'!H28,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E29" s="74" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E29)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G29)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E29)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G29))</f>
@@ -13758,11 +13800,11 @@
       <c r="I29" s="117"/>
       <c r="M29" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O29" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13770,7 +13812,7 @@
       </c>
       <c r="P29" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R29" s="8"/>
     </row>
@@ -14365,11 +14407,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -14377,21 +14419,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>20 champs</v>
+        <v>22 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -14610,7 +14652,7 @@
       </c>
       <c r="D8" s="96">
         <f>M8</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E8" s="97">
         <f>N8</f>
@@ -14618,7 +14660,7 @@
       </c>
       <c r="F8" s="101">
         <f>O8</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -14628,7 +14670,7 @@
       </c>
       <c r="M8" s="1">
         <f>'Sprint 1 - Planification'!AJ18</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1">
         <f>'Sprint 1 - Planification'!AJ19</f>
@@ -14636,7 +14678,7 @@
       </c>
       <c r="O8" s="1">
         <f>SUM(L8:N8)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -14653,7 +14695,7 @@
       </c>
       <c r="D9" s="99" t="str">
         <f t="shared" si="0"/>
-        <v>26h45</v>
+        <v>34h45</v>
       </c>
       <c r="E9" s="100" t="str">
         <f t="shared" si="0"/>
@@ -14661,7 +14703,7 @@
       </c>
       <c r="F9" s="102" t="str">
         <f t="shared" si="0"/>
-        <v>61h15</v>
+        <v>69h15</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -14671,7 +14713,7 @@
       </c>
       <c r="M9" s="1">
         <f>'Sprint 1 - Planification'!AD18</f>
-        <v>1.1145833333333346</v>
+        <v>1.4479166666666676</v>
       </c>
       <c r="N9" s="1">
         <f>'Sprint 1 - Planification'!AD19</f>
@@ -14679,7 +14721,7 @@
       </c>
       <c r="O9" s="1">
         <f>SUM(L9:N9)</f>
-        <v>2.5520833333333375</v>
+        <v>2.8854166666666705</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>66</v>
@@ -14690,7 +14732,7 @@
       </c>
       <c r="R9" s="1">
         <f t="shared" si="1"/>
-        <v>26.75</v>
+        <v>34.75</v>
       </c>
       <c r="S9" s="1">
         <f t="shared" si="1"/>
@@ -14701,7 +14743,7 @@
       </c>
       <c r="V9" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!E8:E42,"Essentielle")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>70</v>
@@ -14721,7 +14763,7 @@
       </c>
       <c r="D10" s="96" t="str">
         <f t="shared" si="0"/>
-        <v>16h00</v>
+        <v>17h00</v>
       </c>
       <c r="E10" s="97" t="str">
         <f t="shared" si="0"/>
@@ -14729,7 +14771,7 @@
       </c>
       <c r="F10" s="101" t="str">
         <f t="shared" si="0"/>
-        <v>49h15</v>
+        <v>50h15</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -14739,7 +14781,7 @@
       </c>
       <c r="M10" s="1">
         <f>'Sprint 2 - Bilan'!V9</f>
-        <v>0.66666666666667596</v>
+        <v>0.7083333333333427</v>
       </c>
       <c r="N10" s="1">
         <f>'Sprint 3 - Bilan'!V9</f>
@@ -14747,7 +14789,7 @@
       </c>
       <c r="O10" s="1">
         <f>SUM(L10:N10)</f>
-        <v>2.0520833333333441</v>
+        <v>2.0937500000000107</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>67</v>
@@ -14758,7 +14800,7 @@
       </c>
       <c r="R10" s="1">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" si="1"/>
@@ -14776,7 +14818,7 @@
       </c>
       <c r="Y10" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!F8:F42,2)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:25" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -14789,15 +14831,15 @@
       </c>
       <c r="D11" s="105">
         <f>M11</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="106">
         <f>N11</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" s="107">
         <f>O11</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -14807,15 +14849,15 @@
       </c>
       <c r="M11" s="1">
         <f>'Sprint 2 - Bilan'!V16</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N11" s="1">
         <f>'Sprint 3 - Bilan'!V16</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O11" s="1">
         <f>N11</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>

</xml_diff>

<commit_message>
arbres ajoutes. prochaine etape:refactoring du code pour avoir un projet plus propre.
</commit_message>
<xml_diff>
--- a/B65_-_Automne_2018_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
+++ b/B65_-_Automne_2018_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="9195" tabRatio="494" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="9195" tabRatio="494" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Planification" sheetId="1" r:id="rId1"/>
@@ -2613,7 +2613,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2728,8 +2727,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="-1018659632"/>
-        <c:axId val="-1018669968"/>
+        <c:axId val="2066470672"/>
+        <c:axId val="2066459248"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2802,11 +2801,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1018659632"/>
-        <c:axId val="-1018669968"/>
+        <c:axId val="2066470672"/>
+        <c:axId val="2066459248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1018659632"/>
+        <c:axId val="2066470672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2849,7 +2848,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1018669968"/>
+        <c:crossAx val="2066459248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2857,7 +2856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1018669968"/>
+        <c:axId val="2066459248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2908,7 +2907,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1018659632"/>
+        <c:crossAx val="2066470672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2922,7 +2921,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3029,7 +3027,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3193,7 +3190,7 @@
                   <c:v>33.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>19.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3212,11 +3209,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-15"/>
-        <c:axId val="-1012901168"/>
-        <c:axId val="-1012900624"/>
+        <c:axId val="2072150912"/>
+        <c:axId val="2072154720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1012901168"/>
+        <c:axId val="2072150912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3259,7 +3256,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1012900624"/>
+        <c:crossAx val="2072154720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3267,7 +3264,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1012900624"/>
+        <c:axId val="2072154720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3318,7 +3315,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1012901168"/>
+        <c:crossAx val="2072150912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3332,7 +3329,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3439,7 +3435,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3737,7 +3732,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3844,7 +3838,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4166,7 +4159,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10924,7 +10916,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="64" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 16 champs à remplir!</v>
+        <v>Attention, il reste 15 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -11021,7 +11013,7 @@
       </c>
       <c r="V9" s="9">
         <f>SUM(G9:G43)</f>
-        <v>0.7083333333333427</v>
+        <v>0.82291666666667573</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
@@ -11069,15 +11061,15 @@
       </c>
       <c r="S10" s="61">
         <f t="array" ref="S10">SUM(($D$9:$D$43=$R10)*$G$9:$G$43)</f>
-        <v>0.7083333333333427</v>
+        <v>0.82291666666667573</v>
       </c>
       <c r="T10" s="62">
         <f t="shared" ref="T10:T11" si="4">S10*24*60</f>
-        <v>1020.0000000000134</v>
+        <v>1185.000000000013</v>
       </c>
       <c r="V10" s="10">
         <f>V9</f>
-        <v>0.7083333333333427</v>
+        <v>0.82291666666667573</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -11133,7 +11125,7 @@
       </c>
       <c r="V11" s="63">
         <f>DAY(V9)*24+HOUR(V9)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -11180,7 +11172,7 @@
       <c r="R12" s="8"/>
       <c r="V12" s="4">
         <f>MINUTE(V9)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
@@ -11229,11 +11221,11 @@
       </c>
       <c r="V13" s="63">
         <f>V11</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="W13" s="4" t="str">
         <f>V13 &amp; " " &amp; U13 &amp; IF(V13 &gt; 1, "s", "")</f>
-        <v>17 heures</v>
+        <v>19 heures</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
@@ -11282,11 +11274,11 @@
       </c>
       <c r="V14" s="4">
         <f>V12</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="W14" s="4" t="str">
         <f>V14 &amp; " " &amp; U14 &amp; IF(V14 &gt; 1, "s", "")</f>
-        <v>0 minute</v>
+        <v>45 minutes</v>
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
@@ -11332,11 +11324,11 @@
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
         <f>IF(V13&gt;0,IF(V14&gt;0,W13&amp;" et "&amp;W14,W13),W14)</f>
-        <v>17 heures</v>
+        <v>19 heures et 45 minutes</v>
       </c>
       <c r="Y15" s="4" t="str">
         <f>V13&amp;"h"&amp;TEXT(V14,"00")</f>
-        <v>17h00</v>
+        <v>19h45</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
@@ -11923,20 +11915,24 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F28),"",'Sprint 1 - Bilan'!F28)</f>
         <v/>
       </c>
-      <c r="G29" s="115"/>
-      <c r="H29" s="116"/>
+      <c r="G29" s="115">
+        <v>0.114583333333333</v>
+      </c>
+      <c r="H29" s="116">
+        <v>0.15</v>
+      </c>
       <c r="I29" s="117"/>
       <c r="M29" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N29" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" s="3" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29" s="3" t="b">
         <f t="shared" si="3"/>
@@ -12535,15 +12531,15 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
@@ -12554,14 +12550,14 @@
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>16 champs</v>
+        <v>15 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -12706,7 +12702,7 @@
       <formula>LEN($B10)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="7">
+  <dataValidations count="7">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nom de tâche trop long" error="Le nom de votre tâche doit être court. _x000a_Un maximum de 72 caractères est mis à votre disposition._x000a_Pour plus de détail, veuillez faire l'ajout de commentaires." promptTitle="Nom de la tâche" prompt="_x000a_Veuillez saisir le nom de la tâche._x000a__x000a_Lorsque pertinent, n'oubliez pas d'ajouter une description de votre tâche sous forme de commentaire." sqref="C9:C43">
       <formula1>0</formula1>
       <formula2>72</formula2>
@@ -13787,13 +13783,13 @@
         <f>IF(LEN('Sprint 1 - Planification'!H28)&lt;&gt;0,'Sprint 1 - Planification'!H28,"")</f>
         <v>Sprint 2</v>
       </c>
-      <c r="E29" s="74" t="str">
+      <c r="E29" s="74">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E29)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G29)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E29)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G29))</f>
-        <v/>
-      </c>
-      <c r="F29" s="78" t="str">
+        <v>0.114583333333333</v>
+      </c>
+      <c r="F29" s="78">
         <f>IF(LEN('Sprint 2 - Bilan'!$H29)&lt;&gt;0,'Sprint 2 - Bilan'!$H29,IF(LEN('Sprint 2 - Bilan'!$F29)=0,"",'Sprint 2 - Bilan'!$F29))</f>
-        <v/>
+        <v>0.15</v>
       </c>
       <c r="G29" s="115"/>
       <c r="H29" s="116"/>
@@ -14763,7 +14759,7 @@
       </c>
       <c r="D10" s="96" t="str">
         <f t="shared" si="0"/>
-        <v>17h00</v>
+        <v>19h45</v>
       </c>
       <c r="E10" s="97" t="str">
         <f t="shared" si="0"/>
@@ -14771,7 +14767,7 @@
       </c>
       <c r="F10" s="101" t="str">
         <f t="shared" si="0"/>
-        <v>50h15</v>
+        <v>53h00</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -14781,7 +14777,7 @@
       </c>
       <c r="M10" s="1">
         <f>'Sprint 2 - Bilan'!V9</f>
-        <v>0.7083333333333427</v>
+        <v>0.82291666666667573</v>
       </c>
       <c r="N10" s="1">
         <f>'Sprint 3 - Bilan'!V9</f>
@@ -14789,7 +14785,7 @@
       </c>
       <c r="O10" s="1">
         <f>SUM(L10:N10)</f>
-        <v>2.0937500000000107</v>
+        <v>2.2083333333333437</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>67</v>
@@ -14800,7 +14796,7 @@
       </c>
       <c r="R10" s="1">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>19.75</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" si="1"/>

</xml_diff>